<commit_message>
Update Example code test
</commit_message>
<xml_diff>
--- a/src/test/resources/testdatafile/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdatafile/ClientsDataExcel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>thaian@mailinator.com</t>
   </si>
@@ -297,7 +297,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -355,6 +355,21 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
@@ -756,7 +771,7 @@
       <c r="B4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="27" t="s">
         <v>41</v>
       </c>
       <c r="D4" s="19" t="s">

</xml_diff>

<commit_message>
Update report and read data test example
</commit_message>
<xml_diff>
--- a/src/test/resources/testdatafile/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdatafile/ClientsDataExcel.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\PERSONAL_PROJECT_AUTO_TEST\SeleniumFrameworkTestNG\src\test\resources\testdatafile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\PERSONAL_PROJECT_AUTO_TEST\AutomationFrameworkSelenium\src\test\resources\testdatafile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27591F7-D338-4623-AEE0-BE5D1A686B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45444FE-19D9-434E-A08F-4419F581FC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3384" yWindow="2208" windowWidth="17280" windowHeight="8880" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>thaian@mailinator.com</t>
   </si>
@@ -159,7 +159,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -234,7 +233,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,11 +260,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -297,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -356,28 +350,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -698,18 +671,18 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="23.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="28.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="15" width="12.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="15" width="17.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="22.5546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="17.0" collapsed="true"/>
-    <col min="7" max="16384" style="15" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="23.33203125" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.5546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.6640625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.6640625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.5546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.88671875" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -771,7 +744,7 @@
       <c r="B4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="20" t="s">
         <v>41</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -787,8 +760,8 @@
       <c r="B5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="16">
-        <v>123456</v>
+      <c r="C5" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>39</v>
@@ -817,13 +790,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="8" width="26.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="8" width="16.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="8" width="14.33203125" collapsed="true"/>
-    <col min="4" max="8" customWidth="true" style="8" width="14.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="8" width="14.0" collapsed="true"/>
-    <col min="10" max="10" style="8" width="8.77734375" collapsed="true"/>
-    <col min="11" max="16384" style="8" width="8.77734375" collapsed="true"/>
+    <col min="1" max="1" width="26.21875" style="8" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.44140625" style="8" customWidth="1" collapsed="1"/>
+    <col min="3" max="8" width="14.33203125" style="8" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14" style="8" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="8.77734375" style="8" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1057,13 +1028,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="26.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="16.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="14.33203125" collapsed="true"/>
-    <col min="4" max="8" customWidth="true" style="2" width="14.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="2" width="14.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="2" width="17.44140625" collapsed="true"/>
-    <col min="11" max="16384" style="2" width="8.77734375" collapsed="true"/>
+    <col min="1" max="1" width="26.21875" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="8" width="14.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14" style="2" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="8.77734375" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update version 1.6.0 PREVIEW
</commit_message>
<xml_diff>
--- a/src/test/resources/testdatafile/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdatafile/ClientsDataExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\PROJECT_FRAMEWORK\AutomationFrameworkSelenium\src\test\resources\testdatafile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL_PROJECT_AUTO_TEST\AutomationFrameworkSelenium\src\test\resources\testdatafile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B150B67-D164-48A8-801B-5EEA66B385EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B8393E-81C1-4498-A33B-932D2E0877FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="23100" windowHeight="13005" activeTab="1" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="3" r:id="rId1"/>
@@ -70,12 +70,6 @@
     <t>20</t>
   </si>
   <si>
-    <t>auto</t>
-  </si>
-  <si>
-    <t>manual</t>
-  </si>
-  <si>
     <t>TESTCASENAME</t>
   </si>
   <si>
@@ -127,48 +121,54 @@
     <t>EXPECTED_URL</t>
   </si>
   <si>
-    <t>admin02@mailinator.com</t>
-  </si>
-  <si>
-    <t>tld01@mailinator.com</t>
-  </si>
-  <si>
     <t>pass</t>
   </si>
   <si>
-    <t>testGetSignInData</t>
-  </si>
-  <si>
     <t>testAddClient</t>
   </si>
   <si>
     <t>Thai Thi Hanh</t>
   </si>
   <si>
-    <t>Admin 02</t>
-  </si>
-  <si>
-    <t>Team Member 01</t>
-  </si>
-  <si>
-    <t>Anh Tester Client 1406A4</t>
-  </si>
-  <si>
-    <t>Anh Tester Client 1406A5</t>
-  </si>
-  <si>
-    <t>Anh Tester Client 1406A6</t>
+    <t>admin@mailinator.com</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>projectmanager@mailinator.com</t>
+  </si>
+  <si>
+    <t>testSignInData</t>
+  </si>
+  <si>
+    <t>VIP</t>
+  </si>
+  <si>
+    <t>PRO</t>
+  </si>
+  <si>
+    <t>Anh Tester</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 0107A7</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 0107A8</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 0107A9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -176,7 +176,15 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -185,14 +193,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -204,14 +212,14 @@
     </font>
     <font>
       <sz val="14"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF0070C0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -219,7 +227,7 @@
       <u/>
       <sz val="14"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -227,13 +235,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -241,7 +249,7 @@
       <u/>
       <sz val="14"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -250,7 +258,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -285,46 +293,47 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -642,68 +651,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF288A0-DB40-4E38-9AAF-ADDED2880E84}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="36.25" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.125" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.5" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.75" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="8.875" style="12" collapsed="1"/>
-    <col min="9" max="16384" width="8.875" style="1" collapsed="1"/>
+    <col min="1" max="1" width="20.21875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.21875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.33203125" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5546875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.44140625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.33203125" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="8.88671875" style="12" collapsed="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>32</v>
-      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>35</v>
-      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>9</v>
-      </c>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -720,77 +768,77 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.25" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="18.21875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.25" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.25" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="5.125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.25" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="18.25" style="2" collapsed="1"/>
+    <col min="1" max="1" width="15.88671875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.77734375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="18.21875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -817,22 +865,22 @@
         <v>12</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
@@ -856,19 +904,19 @@
         <v>30</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
@@ -895,12 +943,12 @@
         <v>13</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="M4" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{ED197778-D3E0-411D-9BE8-9D641596BB30}"/>
     <hyperlink ref="J3" r:id="rId2" xr:uid="{6BB180CC-F100-4639-BD3A-B7B33CC640F9}"/>

</xml_diff>